<commit_message>
fix the repeat-rows pipe
</commit_message>
<xml_diff>
--- a/out2.xlsx
+++ b/out2.xlsx
@@ -106,7 +106,7 @@
     <t>Да</t>
   </si>
   <si>
-    <t xml:space="preserve"> : </t>
+    <t xml:space="preserve">Замер: </t>
   </si>
   <si>
     <t/>
@@ -150,7 +150,8 @@
     <t>/data/www/xls-report/alex.jpg</t>
   </si>
   <si>
-    <t>Дата: 2018-5-15, GPS: 48.800744, 44.726850</t>
+    <t>Дата: 2018-5-16
+GPS: 48.800744, 44.726850</t>
   </si>
   <si>
     <t>Текст шага инспекции 2</t>
@@ -175,7 +176,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -218,12 +219,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="9"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -239,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -382,46 +377,14 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
@@ -480,12 +443,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" wrapText="1" shrinkToFit="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1" shrinkToFit="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1" shrinkToFit="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -499,12 +456,6 @@
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -574,13 +525,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -618,13 +569,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>6</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -663,7 +614,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z994"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -1597,105 +1548,105 @@
       </c>
       <c r="B43"/>
     </row>
-    <row r="44" ht="87" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
+    <row r="44" ht="147" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
+      <c r="B44" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+    </row>
+    <row r="45" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B46"/>
-    </row>
-    <row r="47" ht="87" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+      <c r="B45"/>
+    </row>
+    <row r="46" ht="147" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="21" t="s">
+      <c r="B46" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+    </row>
+    <row r="47" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B49"/>
-    </row>
-    <row r="50" ht="87" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+      <c r="B47"/>
+    </row>
+    <row r="48" ht="147" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="21" t="s">
+      <c r="B48" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="1"/>
+    </row>
+    <row r="49" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51"/>
     </row>
     <row r="52" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
     <row r="53" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B54"/>
-    </row>
-    <row r="55" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+      <c r="A53" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B53" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
+    <row r="54" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B54" s="23"/>
+    </row>
+    <row r="55" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="24"/>
+      <c r="B55" s="23"/>
+    </row>
+    <row r="56" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="24"/>
+      <c r="B56" s="23"/>
+    </row>
+    <row r="57" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="24"/>
+      <c r="B57" s="23"/>
     </row>
     <row r="58" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
-      <c r="B58" s="25"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="23"/>
     </row>
     <row r="59" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
-      <c r="B59" s="25"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
     </row>
     <row r="60" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
-      <c r="B60" s="25"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
     </row>
     <row r="61" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
-      <c r="B61" s="25"/>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
     </row>
     <row r="62" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="27"/>
-      <c r="B62" s="28"/>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
     </row>
     <row r="63" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
@@ -1713,17 +1664,89 @@
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
     </row>
-    <row r="67" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" ht="12.75" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-    </row>
-    <row r="68" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+    </row>
+    <row r="68" ht="12.75" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-    </row>
-    <row r="69" ht="12.75" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1"/>
+    </row>
+    <row r="69" ht="12.75" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
     </row>
     <row r="70" ht="12.75" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
@@ -27597,34 +27620,6 @@
       <c r="Y993" s="1"/>
       <c r="Z993" s="1"/>
     </row>
-    <row r="994" ht="12.75" customHeight="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A994" s="1"/>
-      <c r="B994" s="1"/>
-      <c r="C994" s="1"/>
-      <c r="D994" s="1"/>
-      <c r="E994" s="1"/>
-      <c r="F994" s="1"/>
-      <c r="G994" s="1"/>
-      <c r="H994" s="1"/>
-      <c r="I994" s="1"/>
-      <c r="J994" s="1"/>
-      <c r="K994" s="1"/>
-      <c r="L994" s="1"/>
-      <c r="M994" s="1"/>
-      <c r="N994" s="1"/>
-      <c r="O994" s="1"/>
-      <c r="P994" s="1"/>
-      <c r="Q994" s="1"/>
-      <c r="R994" s="1"/>
-      <c r="S994" s="1"/>
-      <c r="T994" s="1"/>
-      <c r="U994" s="1"/>
-      <c r="V994" s="1"/>
-      <c r="W994" s="1"/>
-      <c r="X994" s="1"/>
-      <c r="Y994" s="1"/>
-      <c r="Z994" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A2:B2"/>
@@ -27640,9 +27635,9 @@
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A51:B51"/>
   </mergeCells>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>